<commit_message>
Research notes + PRISMA integ
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -464,7 +464,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The title of the paper is:
+          <t>Based on the text provided, the title of the paper is:
 **TYCOV: An Open-Source, Year-Long Behavioral Study of Human Ability to Detect AI-Generated Images**</t>
         </is>
       </c>
@@ -482,12 +482,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1,217 unique participants (humans) using a web application.</t>
+          <t>1,217 unique participants of a public web application who performed a visual classification task.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
@@ -499,12 +499,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Performing forced-choice classifications on a balanced set of real and AI-generated images to detect which ones were generated by AI.</t>
+          <t>Forced-choice classification of images, determining whether each image was real or AI-generated.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
@@ -528,12 +528,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The accuracy of human detection of AI-generated images, measured as aggregate accuracy, class-conditional accuracies (for real vs. AI images), and longitudinal trends in accuracy over 55 weeks.</t>
+          <t>The accuracy of human detection of AI-generated versus real images, including aggregate accuracy, class-conditional accuracies, and longitudinal trends in accuracy over 55 weeks.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The research is an observational study that collected data from a large cohort of 1,217 participants over a 55-week period. This design prospectively gathers data to measure outcomes and trends in a defined group over time, which is characteristic of a cohort study. It is not a Randomized Controlled Trial as there was no random assignment to an intervention, thus it receives a 'Medium' quality score according to the rubric.</t>
+          <t>The study is an observational behavioral study where data was collected from a self-selected, non-randomized group of participants via a public web application. This design most closely resembles a cross-sectional study, as it measures the ability of a sample population over a period without a controlled intervention or a defined cohort being followed over time. According to the provided rubric, a cross-sectional study is assigned a 'Low' quality score.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -582,7 +582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -623,59 +623,59 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Participants identify Real images (67.8%) more reliably than AI images (52.8%).</t>
+          <t>Total trial-level responses: N = 60,123 (from n = 1,217 unique participants; mean ≈49.4 trials per participant).</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cluster-aware participant-level analyses were conducted and confirm the descriptive asymmetry (higher accuracy for Real images than AI images).</t>
+          <t>Aggregate accuracy: 60.3%.</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>the overall pattern [of weekly mean accuracy] indicates a modest upward drift.</t>
+          <t>Class-conditional accuracies: preal = 0.678 (67.8%) for ground-truth Real images; pai = 0.528 (52.8%) for ground-truth AI images.</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>The (AI →Real) off-diagonal cell is larger than the reverse, confirming an authenticity bias where AI images are more often labeled Real than Real images are labeled AI.</t>
+          <t>Participants identify Real images (67.8%) more reliably than AI images (52.8%).</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -683,37 +683,82 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>unaided human detection of AI-generated images is modest (60.3%) and asymmetric: observers better detect real images than AI images.</t>
+          <t>cluster-aware participant-level analyses were conducted and confirm the descriptive asymmetry (higher accuracy for Real images than AI images).</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>verified</t>
+          <t>unverified</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>the overall pattern indicates a modest upward drift.</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>unverified</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>The (AI →Real) off-diagonal cell is larger than the reverse, confirming an authenticity bias where AI images are more often labeled Real than Real images are labeled AI.</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>unverified</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>unaided human detection of AI-generated images is modest (60.3%) and asymmetric: observers better detect real images than AI images.</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>unverified</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>Human observers alone are only modestly reliable detectors of synthetic imagery and tend to err toward assuming authenticity.</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B11" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>verified</t>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>unverified</t>
         </is>
       </c>
     </row>

</xml_diff>